<commit_message>
updated the results page and the reuslts with updated code including dense_rank and more efficient code. And adjusted name spelling from the first competition blog post
</commit_message>
<xml_diff>
--- a/assets/data/Result_no1.xlsx
+++ b/assets/data/Result_no1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R_blogg\lagerlof_org\km\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF4C045B-CDF6-4262-ABD7-40CF57CAFE53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03AD9F9E-3D12-4066-A50E-E573423C11E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{0837BD7A-19EF-40B4-956C-F4752F5E0E49}"/>
   </bookViews>
@@ -74,9 +74,6 @@
     <t>Gustaf Falkner</t>
   </si>
   <si>
-    <t>Jakob Symne</t>
-  </si>
-  <si>
     <t>Hugo Wik</t>
   </si>
   <si>
@@ -105,6 +102,9 @@
   </si>
   <si>
     <t>Natalie Wramner</t>
+  </si>
+  <si>
+    <t>Jakob Stymne</t>
   </si>
 </sst>
 </file>
@@ -459,7 +459,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -480,7 +480,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -513,7 +513,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -579,7 +579,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -612,7 +612,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -623,7 +623,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -634,7 +634,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -645,7 +645,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -667,7 +667,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>17</v>
@@ -678,7 +678,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B20">
         <v>18</v>
@@ -689,7 +689,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21">
         <v>19</v>
@@ -700,7 +700,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22">
         <v>20</v>
@@ -719,6 +719,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="dokument" ma:contentTypeID="0x0101004EF54028F6CBCA468BE651ABA28D50BB" ma:contentTypeVersion="10" ma:contentTypeDescription="Skapa ett nytt dokument." ma:contentTypeScope="" ma:versionID="ecf9ae7cb170956cb2a369b5233e02ad">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="db6f6976-153c-41c0-925b-40783e97e3a7" xmlns:ns4="d002855e-ed1c-4d8d-9d54-9af106433259" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c6d00720273d804f5936139e4fe0db26" ns3:_="" ns4:_="">
     <xsd:import namespace="db6f6976-153c-41c0-925b-40783e97e3a7"/>
@@ -921,12 +927,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -937,6 +937,15 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CFD49A51-A312-443A-AEB2-8516D440E0C1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{453CB572-EF92-45A6-A68F-FADD33720D74}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -955,15 +964,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CFD49A51-A312-443A-AEB2-8516D440E0C1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F3CA5DA-AFD4-4FAA-993E-F5B6AFC2E9C9}">
   <ds:schemaRefs>

</xml_diff>